<commit_message>
Update scripts and documentation for edits
</commit_message>
<xml_diff>
--- a/nanni_maize_2022/documentation/transcriptome_evaluation_counting.xlsx
+++ b/nanni_maize_2022/documentation/transcriptome_evaluation_counting.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="249">
   <si>
     <t xml:space="preserve">Analysis</t>
   </si>
@@ -78,7 +78,9 @@
   <si>
     <t xml:space="preserve">Correct the gene_id values of the GTF output from SQANTI QC to match the gene_id values associated with the transcripts in the classification file
 ** Need to do this to allow to correctly associated isoforms from the same gene or putative novel/fusion loci
-Copy output GTF to HPC</t>
+Copy output GTF to HPC
+Contains 48950 transcripts, 14877 genes/loci (1531 novel loci, 13346 annotated)
+Of the novel loci there are 279 antisense transcripts in 187 novel antisense genes</t>
   </si>
   <si>
     <t xml:space="preserve">$SCRIPTS/correct_SQANTI_QC_GTF_gene_id_02avn.py
@@ -88,7 +90,8 @@
     <t xml:space="preserve">$SCRIPTS/run_correct_baseline_SQANTI_QC_GTF_gene_id.sh</t>
   </si>
   <si>
-    <t xml:space="preserve">$PROJ/sqanti_post_filter_b73/sqanti_b73_filtered_corrected.gtf</t>
+    <t xml:space="preserve">$PROJ/sqanti_post_filter_b73/sqanti_b73_filtered_corrected.gtf
+** NOTE THIS IS A COPY FROM HPC: $PROJ/compare_b73_2_mo17/sqanti_post_filter/sqanti_filtered_corrected.gtf</t>
   </si>
   <si>
     <t xml:space="preserve">$PROJ/sqanti_post_filter_b73/sqanti_b73_filtered_corrected_associated_gene.gtf
@@ -104,6 +107,27 @@
   </si>
   <si>
     <t xml:space="preserve">Quantify genes and novel/fusion loci with htseq</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Quantify genes and novel/fusion loci with htseq (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">14877 genes/loci)</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">htseq/0.11.2
@@ -229,7 +253,31 @@
     <t xml:space="preserve">Event analysis annotations of curated transcriptome</t>
   </si>
   <si>
-    <t xml:space="preserve">Get event analysis annotations for concatenated GTF files of representative reference annotations for FSM/ISM and NIC/NNC monoexon filtered transcripts (curated transcriptome)</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Concatenated GTF files of:
+1) Representative reference annotations for FSM/ISM (19251 transcripts and 12033 genes)
+2) NIC/NNC monoexon filtered transcripts (12392 transcripts and 4786 genes)
+(31643 total transcripts, 12604 total genes)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+Get event analysis annotations
+** EA dropped Mt and Pt chromosomes (89 transcripts, 89 genes) BUT these are added back in later</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">$SCRIPTS/run_combine_GTFs_and_convert_GFF3_02avn.sh
@@ -241,9 +289,9 @@
 $PROJ/nic_nnc_monoexon_filter/sqanti_b73_nic_nnc_monoexon_filter_pb2fbgn.gt</t>
   </si>
   <si>
-    <t xml:space="preserve">$PROJ/sqanti_classification_category_subse/ZMtr_from_pbID_fsm_ism_plus_nic_nnc_monoexon_filter.gtf
-$PROJ/sqanti_classification_category_subse/ZMtr_from_pbID_fsm_ism_plus_nic_nnc_monoexon_filter.EA_converted.gff
-$PROJ/sqanti_classification_category_subse/ZMtr_from_pbID_fsm_ism_plus_nic_nnc_monoexon_filter.EA_converted.gff.db
+    <t xml:space="preserve">$PROJ/sqanti_classification_category_subset/ZMtr_from_pbID_fsm_ism_plus_nic_nnc_monoexon_filter.gtf
+$PROJ/sqanti_classification_category_subset/ZMtr_from_pbID_fsm_ism_plus_nic_nnc_monoexon_filter.EA_converted.gff
+$PROJ/sqanti_classification_category_subset/ZMtr_from_pbID_fsm_ism_plus_nic_nnc_monoexon_filter.EA_converted.gff.db
 $PROJ/sqanti_classification_category_subset/EA_annotations/*</t>
   </si>
   <si>
@@ -507,7 +555,8 @@
 $PROJ/RNAseq_rsem_fsm_ism_nic_nnc_consol_junc/fsm_ism_nic_nnc_consol_junc.isoforms_lengths.txt</t>
   </si>
   <si>
-    <t xml:space="preserve">Flag on/off</t>
+    <t xml:space="preserve">Flag on/off
+LOOKS LIKE ISOFORMS ONLY</t>
   </si>
   <si>
     <t xml:space="preserve">Flag on/off for all genotype_treatment groups (10 total):
@@ -557,7 +606,8 @@
 10     8360</t>
   </si>
   <si>
-    <t xml:space="preserve">Prep files for tappAS</t>
+    <t xml:space="preserve">Prep files for tappAS
+ISOFORMS ONLY???</t>
   </si>
   <si>
     <t xml:space="preserve">Using on/off flags (TPM&gt;5 in at least 50% of reps) select transcripts that are detected in at least 2 samples
@@ -689,9 +739,40 @@
     <t xml:space="preserve">$PROJ/RNAseq_rsem_fsm_ism_nic_nnc_consol_junc/final_maize.annotation_output4TAPPAS_mod_consol.gff</t>
   </si>
   <si>
-    <t xml:space="preserve">tappAS: Amb vs. ozone
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">tappAS: Amb vs. ozone
 Import data into tappAS and run DEA/DIU
-!! Only ran DEA on genes and DIU so far</t>
+!! Only ran DEA on genes and DIU so far
+[</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">note input into tappas is isoform level and output from tappas is gene level</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">]</t>
+    </r>
   </si>
   <si>
     <r>
@@ -836,7 +917,40 @@
 Zm00001d000070 example in NC338 of 2 xcrpt, 1 with intron retention from PB that show DIU and major isoform switching</t>
   </si>
   <si>
-    <t xml:space="preserve">Combine Amb vs. Oz tappAS results</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Combine Amb vs. Oz tappAS results
+Tappas outputs BOTH isoform and gene results!
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">* if at least 1 isoform for a gene is ‘on’ (tpm 5 in at least 50% of the reps) then the gene is on: flag_&amp;geno._&amp;trt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.
+</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Combine tappAS results for all genotypes with on/offs and count
@@ -853,7 +967,13 @@
 1       86
 2       15
 3        1
-** The 1 gene with 3 is Zm00001d054001 with Hp301, Mo17, and NC338 - all have a change of expression &gt;25</t>
+** The 1 gene with 3 is Zm00001d054001 with Hp301, Mo17, and NC338 - all have a change of expression &gt;25
+Total genes in each DIU file (multitranscript genes detected in each genotype)
+B73_tappAS_DIUGene_Transcripts.tsv 2874
+C123_tappAS_DIUGene_Transcripts.tsv 2941
+Hp301_tappAS_DIUGene_Transcripts.tsv 2696
+Mo17_tappAS_DIUGene_Transcripts.tsv 2961
+NC338_tappAS_DIUGene_Transcripts.tsv 2966</t>
   </si>
   <si>
     <t xml:space="preserve">${SCRIPTS}/merge_tappas_DEA_results.py
@@ -1179,7 +1299,10 @@
     <t xml:space="preserve">${SCRIPTS}/run_plot_maize_PB_groups_UpSet.sh</t>
   </si>
   <si>
-    <t xml:space="preserve">~/mclab/SHARE/McIntyre_Lab/useful_maize_info/RefGenV4/B73_v4_geneIDs_geneNames_02amm.txt</t>
+    <t xml:space="preserve">~/mclab/SHARE/McIntyre_Lab/useful_maize_info/RefGenV4/B73_v4_geneIDs_geneNames_02amm.txt
+${TAPPAS}/all_genotype_flag_tappas_DE_gene_results.csv \
+ ${IND}/flag_on_off_rsem_expression_isoforms_TPM_5_full_table.tsv \
+ ${DIST}/zmtr_fsm_ism_nic_nnc_transcript_id_2_gene_id.csv </t>
   </si>
   <si>
     <t xml:space="preserve">${OUTD}/zmtr_fsm_ism_nic_nnc_consol_${GENO}_DE_pval_hist.png
@@ -1349,6 +1472,76 @@
   <si>
     <t xml:space="preserve">${SCRIPTS}/plot_IR_isoform_expression.py</t>
   </si>
+  <si>
+    <t xml:space="preserve">files and tables containing all results!!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rsem-star-tappas DIU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mclab/SHARE/McIntyre_Lab/maize_ozone_FINAL/2018/PacBio/RNAseq_rsem_fsm_ism_nic_nnc_consol_junc/tappas_output_TMM_norm_1CPMfilter
+all_genotype_flag_tappas_DIU_gene_results_atLeast1geno_DIU_majorIsoformSwitch_w_GO.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rsem-star-tappas DE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mclab/SHARE/McIntyre_Lab/maize_ozone_FINAL/2018/PacBio/RNAseq_rsem_fsm_ism_nic_nnc_consol_junc/tappas_output_TMM_norm_1CPMfilter
+all_genotype_flag_tappas_DE_gene_results_w_GO.csv
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cvrg_cnts_shrtRead,
+By genotype
+With means across reps for weighted TPM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/mclab/SHARE/McIntyre_Lab/maize_ozone_FINAL/make_combination_flag_file/cvrg_shrtRead_tpm_&amp;geno._sbys.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cvrg_cnts_ccs, 
+By genotype
+With means across reps for weighted TPM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/mclab/SHARE/McIntyre_Lab/maize_ozone_FINAL/make_combination_flag_file/design_&amp;geno._shrtRd.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flag file both ccs and shrtRead
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">geneID
+flag_b73_reference_gene
+flag_assembled_transcript = 1 if in gene in sqanti gtf
+flag_assembled_fusion_transcript = 1 if geneID is 2 genes catted together
+flag_assembled_novel_transcript = 1 if novel from sqanti
+flag_in_cvrg_cnts_bed = 1 if gene represented in fusion bed file 
+flag_multigene
+For shortReads only:
+flag_&amp;geno._amb_on = 1 if &gt;= tpm5 in50% of amb reps
+flag_&amp;geno._ele_on = 1 if &gt;= tpm5 in50% of amb reps
+flag_analyze_&amp;geno. = 1 if on in either amb or ele
+For ccs reads:
+flag_detect_ccs_&amp;geno._amb_gt0 = 1 if reads in region &gt; 0 
+flag_detect_ccs_&amp;geno._ele_gt0 = 1 if reads in region &gt; 0 
+flag_detect_ccs_&amp;geno._gt0 = 1 if detected in either amb or ele for &amp;geno
+For shortReads:
+flag_detect_shrtRd_&amp;geno._amb_gt0 = 1 if reads in region &gt; 0
+flag_detect_shrtRd_&amp;geno._ele_gt0 = 1 if reads in region &gt; 0
+flag_detect_shrtRd_&amp;geno._gt0 = 1 if detected in either amb or ele for &amp;geno
+Below f2 lags from /SHARE/McIntyre_Lab/useful_maize_info/gene_lists/Hoopes_2018/Zea_mays_Hoopes_2018_orthogroup_para_flag.csv
+flag_zea_mays_paralog_hoopes 
+Orthgroup_hoopes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">make.combo_flags_shrtRd_ccs
+mclab/SHARE/McIntyre_Lab/maize_ozone_FINAL/make_combination_flag_file/combination_flag_file_shrtRd_ccs_hoopes.csv
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stack cc  for fig [mean exp box plot for genes detected in X num of genos]</t>
+  </si>
 </sst>
 </file>
 
@@ -1357,7 +1550,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1419,6 +1612,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -1430,8 +1637,16 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1442,6 +1657,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFDDDDDD"/>
         <bgColor rgb="FFCCFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -1487,7 +1708,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="29">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1524,11 +1745,15 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1548,6 +1773,22 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1556,7 +1797,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1565,6 +1810,18 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1647,26 +1904,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J1048576"/>
+  <dimension ref="A1:J111"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E47" activeCellId="0" sqref="E47"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="44.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="62.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="32.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="30.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="37.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="37.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="67.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="61.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="38.66"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="1"/>
@@ -1676,7 +1933,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" s="4" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -1690,7 +1947,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" s="4" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="1"/>
@@ -1700,7 +1957,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" s="4" customFormat="true" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="4" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
       <c r="B4" s="2" t="s">
         <v>2</v>
@@ -1714,7 +1971,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" s="4" customFormat="true" ht="86.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" s="4" customFormat="true" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
       <c r="B5" s="2" t="s">
         <v>4</v>
@@ -1730,7 +1987,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="C6" s="1"/>
@@ -1740,7 +1997,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="4"/>
       <c r="C7" s="1"/>
@@ -1750,7 +2007,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -1776,12 +2033,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" s="4" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="10" s="7" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="8"/>
       <c r="G10" s="8"/>
     </row>
-    <row r="11" s="7" customFormat="true" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" s="7" customFormat="true" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
         <v>15</v>
       </c>
@@ -1807,8 +2064,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" s="7" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="13" s="7" customFormat="true" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" s="7" customFormat="true" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="s">
         <v>23</v>
       </c>
@@ -1816,838 +2073,838 @@
         <v>24</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" s="7" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="15" s="7" customFormat="true" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="7" t="s">
         <v>23</v>
       </c>
       <c r="B15" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>28</v>
-      </c>
       <c r="G15" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" s="7" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="17" s="7" customFormat="true" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" s="7" customFormat="true" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" s="7" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="19" s="7" customFormat="true" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" s="7" customFormat="true" ht="191.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" s="7" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="21" s="7" customFormat="true" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="7" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="22" s="4" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="23" s="4" customFormat="true" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" s="4" customFormat="true" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" s="4" t="s">
         <v>53</v>
       </c>
+      <c r="C23" s="9" t="s">
+        <v>54</v>
+      </c>
       <c r="E23" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="24" s="4" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="25" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="27" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="201.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" s="9" t="s">
+      <c r="B29" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="D29" s="9" t="s">
+      <c r="C29" s="10" t="s">
         <v>60</v>
       </c>
+      <c r="D29" s="10" t="s">
+        <v>61</v>
+      </c>
       <c r="E29" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F29" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="G29" s="9" t="s">
+      <c r="F29" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="H29" s="9" t="s">
+      <c r="G29" s="10" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H29" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="7"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
       <c r="E30" s="7"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
     </row>
     <row r="31" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="32" s="4" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="33" s="7" customFormat="true" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="33" s="7" customFormat="true" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="34" s="7" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="35" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="36" s="7" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="37" s="10" customFormat="true" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="10" t="s">
+    <row r="36" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="37" s="11" customFormat="true" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B37" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="C37" s="10" t="s">
+      <c r="B37" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="D37" s="10" t="s">
+      <c r="C37" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E37" s="10" t="s">
+      <c r="D37" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="F37" s="10" t="s">
+      <c r="E37" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="G37" s="10" t="s">
+      <c r="F37" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="H37" s="10" t="s">
+      <c r="G37" s="11" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="38" s="7" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="39" s="7" customFormat="true" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H37" s="11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="39" s="7" customFormat="true" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="40" s="7" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="41" s="7" customFormat="true" ht="270.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="40" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="41" s="7" customFormat="true" ht="225.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="42" s="11" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="43" s="4" customFormat="true" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="42" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="43" s="4" customFormat="true" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="44" s="4" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="45" s="7" customFormat="true" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="44" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="45" s="7" customFormat="true" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="7" t="s">
         <v>23</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="46" s="4" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="47" s="7" customFormat="true" ht="214.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="47" s="7" customFormat="true" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="7" t="s">
         <v>23</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="48" s="11" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="49" s="12" customFormat="true" ht="314.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="12" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="48" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="49" s="13" customFormat="true" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C49" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="D49" s="13" t="s">
+      <c r="C49" s="14" t="s">
         <v>109</v>
       </c>
+      <c r="D49" s="14" t="s">
+        <v>110</v>
+      </c>
       <c r="E49" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="F49" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="G49" s="14" t="s">
+      <c r="F49" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="H49" s="14"/>
-      <c r="I49" s="14"/>
-    </row>
-    <row r="51" s="16" customFormat="true" ht="337.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="3" t="s">
+      <c r="G49" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="H49" s="15"/>
+      <c r="I49" s="15"/>
+    </row>
+    <row r="51" s="19" customFormat="true" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B51" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C51" s="13" t="s">
+      <c r="B51" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="D51" s="13" t="s">
+      <c r="C51" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="E51" s="3" t="s">
+      <c r="D51" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="F51" s="3" t="s">
+      <c r="E51" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="G51" s="3" t="s">
+      <c r="F51" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="H51" s="3" t="s">
+      <c r="G51" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="I51" s="15"/>
-      <c r="J51" s="15"/>
-    </row>
-    <row r="52" s="16" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H51" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="I51" s="18"/>
+      <c r="J51" s="18"/>
+    </row>
+    <row r="52" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
-      <c r="C52" s="13"/>
-      <c r="D52" s="13"/>
+      <c r="C52" s="14"/>
+      <c r="D52" s="14"/>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
-      <c r="I52" s="15"/>
-      <c r="J52" s="15"/>
-    </row>
-    <row r="53" s="9" customFormat="true" ht="236.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="9" t="s">
+      <c r="I52" s="20"/>
+      <c r="J52" s="20"/>
+    </row>
+    <row r="53" s="22" customFormat="true" ht="214.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="B53" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="C53" s="3" t="s">
+      <c r="B53" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="D53" s="9" t="s">
+      <c r="C53" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="E53" s="3" t="s">
+      <c r="D53" s="22" t="s">
         <v>123</v>
       </c>
-      <c r="F53" s="9" t="s">
+      <c r="E53" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="G53" s="9" t="s">
+      <c r="F53" s="22" t="s">
         <v>125</v>
       </c>
-      <c r="H53" s="9" t="s">
+      <c r="G53" s="22" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="54" s="16" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H53" s="22" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="54" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
-      <c r="C54" s="13"/>
-      <c r="D54" s="13"/>
+      <c r="C54" s="14"/>
+      <c r="D54" s="14"/>
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
-      <c r="I54" s="15"/>
-      <c r="J54" s="15"/>
-    </row>
-    <row r="55" s="16" customFormat="true" ht="252.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I54" s="20"/>
+      <c r="J54" s="20"/>
+    </row>
+    <row r="55" s="21" customFormat="true" ht="252.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="C55" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="D55" s="13" t="s">
+      <c r="C55" s="14" t="s">
         <v>129</v>
+      </c>
+      <c r="D55" s="14" t="s">
+        <v>130</v>
       </c>
       <c r="E55" s="3"/>
       <c r="F55" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H55" s="3"/>
-      <c r="I55" s="15"/>
-      <c r="J55" s="15"/>
-    </row>
-    <row r="56" s="16" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I55" s="20"/>
+      <c r="J55" s="20"/>
+    </row>
+    <row r="56" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
-      <c r="C56" s="13"/>
-      <c r="D56" s="13"/>
+      <c r="C56" s="14"/>
+      <c r="D56" s="14"/>
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
-      <c r="I56" s="15"/>
-      <c r="J56" s="15"/>
-    </row>
-    <row r="57" s="16" customFormat="true" ht="303.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I56" s="20"/>
+      <c r="J56" s="20"/>
+    </row>
+    <row r="57" s="21" customFormat="true" ht="258.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="C57" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="D57" s="13" t="s">
+      <c r="C57" s="14" t="s">
         <v>134</v>
+      </c>
+      <c r="D57" s="14" t="s">
+        <v>135</v>
       </c>
       <c r="E57" s="3"/>
       <c r="F57" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="I57" s="15"/>
-      <c r="J57" s="15"/>
-    </row>
-    <row r="58" s="16" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>138</v>
+      </c>
+      <c r="I57" s="20"/>
+      <c r="J57" s="20"/>
+    </row>
+    <row r="58" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
-      <c r="C58" s="13"/>
-      <c r="D58" s="13"/>
+      <c r="C58" s="14"/>
+      <c r="D58" s="14"/>
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
-      <c r="I58" s="15"/>
-      <c r="J58" s="15"/>
-    </row>
-    <row r="59" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I58" s="20"/>
+      <c r="J58" s="20"/>
+    </row>
+    <row r="59" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
-      <c r="C59" s="13"/>
-      <c r="D59" s="13"/>
+      <c r="C59" s="14"/>
+      <c r="D59" s="14"/>
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
       <c r="G59" s="3"/>
       <c r="H59" s="3"/>
-      <c r="I59" s="15"/>
-      <c r="J59" s="15"/>
-    </row>
-    <row r="60" s="16" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I59" s="20"/>
+      <c r="J59" s="20"/>
+    </row>
+    <row r="60" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
-      <c r="C60" s="13"/>
-      <c r="D60" s="13"/>
+      <c r="C60" s="14"/>
+      <c r="D60" s="14"/>
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
       <c r="G60" s="3"/>
       <c r="H60" s="3"/>
-      <c r="I60" s="15"/>
-      <c r="J60" s="15"/>
-    </row>
-    <row r="61" s="9" customFormat="true" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="9" t="s">
+      <c r="I60" s="20"/>
+      <c r="J60" s="20"/>
+    </row>
+    <row r="61" s="22" customFormat="true" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B61" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="C61" s="9" t="s">
+      <c r="B61" s="22" t="s">
         <v>139</v>
       </c>
-      <c r="D61" s="9" t="s">
+      <c r="C61" s="22" t="s">
         <v>140</v>
       </c>
-      <c r="E61" s="9" t="s">
+      <c r="D61" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="F61" s="9" t="s">
+      <c r="E61" s="22" t="s">
         <v>142</v>
       </c>
-      <c r="G61" s="9" t="s">
+      <c r="F61" s="22" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="62" s="9" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="63" s="18" customFormat="true" ht="388.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="9" t="s">
+      <c r="G61" s="22" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="62" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="63" s="24" customFormat="true" ht="281.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B63" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="C63" s="17" t="s">
+      <c r="B63" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="D63" s="17"/>
-      <c r="E63" s="9"/>
-      <c r="F63" s="9" t="s">
+      <c r="C63" s="23" t="s">
         <v>146</v>
       </c>
-      <c r="G63" s="9" t="s">
+      <c r="D63" s="23"/>
+      <c r="E63" s="10"/>
+      <c r="F63" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="H63" s="9" t="s">
+      <c r="G63" s="10" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="64" s="16" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H63" s="10" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="64" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
-      <c r="C64" s="13"/>
-      <c r="D64" s="13"/>
+      <c r="C64" s="14"/>
+      <c r="D64" s="14"/>
       <c r="E64" s="3"/>
       <c r="F64" s="3"/>
       <c r="G64" s="3"/>
       <c r="H64" s="3"/>
-      <c r="I64" s="15"/>
-      <c r="J64" s="15"/>
-    </row>
-    <row r="65" s="16" customFormat="true" ht="316.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="3" t="s">
+      <c r="I64" s="20"/>
+      <c r="J64" s="20"/>
+    </row>
+    <row r="65" s="19" customFormat="true" ht="314.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B65" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="C65" s="13" t="s">
+      <c r="B65" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="D65" s="13" t="s">
+      <c r="C65" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="E65" s="13" t="s">
+      <c r="D65" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="F65" s="3" t="s">
+      <c r="E65" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="G65" s="3" t="s">
+      <c r="F65" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="H65" s="3" t="s">
+      <c r="G65" s="16" t="s">
         <v>155</v>
       </c>
-      <c r="I65" s="15"/>
-      <c r="J65" s="15"/>
-    </row>
-    <row r="66" s="16" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H65" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="I65" s="18"/>
+      <c r="J65" s="18"/>
+    </row>
+    <row r="66" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
-      <c r="C66" s="13"/>
-      <c r="D66" s="13"/>
+      <c r="C66" s="14"/>
+      <c r="D66" s="14"/>
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
       <c r="G66" s="3"/>
       <c r="H66" s="3"/>
-      <c r="I66" s="15"/>
-      <c r="J66" s="15"/>
-    </row>
-    <row r="67" s="18" customFormat="true" ht="216" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="9" t="s">
+      <c r="I66" s="20"/>
+      <c r="J66" s="20"/>
+    </row>
+    <row r="67" s="24" customFormat="true" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B67" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="C67" s="17" t="s">
+      <c r="B67" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="D67" s="17"/>
-      <c r="E67" s="9"/>
-      <c r="F67" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="G67" s="9" t="s">
+      <c r="C67" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="D67" s="23"/>
+      <c r="E67" s="10"/>
+      <c r="F67" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="H67" s="9" t="s">
+      <c r="G67" s="10" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="68" s="18" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="9"/>
-      <c r="B68" s="9"/>
-      <c r="C68" s="17"/>
-      <c r="D68" s="17"/>
-      <c r="E68" s="9"/>
-      <c r="F68" s="9"/>
-      <c r="G68" s="9"/>
-      <c r="H68" s="9"/>
-    </row>
-    <row r="69" s="16" customFormat="true" ht="214.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H67" s="10" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="68" s="24" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="10"/>
+      <c r="B68" s="10"/>
+      <c r="C68" s="23"/>
+      <c r="D68" s="23"/>
+      <c r="E68" s="10"/>
+      <c r="F68" s="10"/>
+      <c r="G68" s="10"/>
+      <c r="H68" s="10"/>
+    </row>
+    <row r="69" s="21" customFormat="true" ht="191.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="C69" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="D69" s="13" t="s">
+      <c r="C69" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="E69" s="13" t="s">
+      <c r="D69" s="14" t="s">
         <v>161</v>
       </c>
+      <c r="E69" s="14" t="s">
+        <v>162</v>
+      </c>
       <c r="F69" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H69" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="I69" s="15"/>
-      <c r="J69" s="15"/>
-    </row>
-    <row r="70" s="16" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>165</v>
+      </c>
+      <c r="I69" s="20"/>
+      <c r="J69" s="20"/>
+    </row>
+    <row r="70" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
-      <c r="C70" s="13"/>
-      <c r="D70" s="13"/>
-      <c r="E70" s="13"/>
+      <c r="C70" s="14"/>
+      <c r="D70" s="14"/>
+      <c r="E70" s="14"/>
       <c r="F70" s="3"/>
       <c r="G70" s="3"/>
       <c r="H70" s="3"/>
-      <c r="I70" s="15"/>
-      <c r="J70" s="15"/>
-    </row>
-    <row r="71" s="16" customFormat="true" ht="270.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I70" s="20"/>
+      <c r="J70" s="20"/>
+    </row>
+    <row r="71" s="21" customFormat="true" ht="270.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="C71" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="D71" s="13" t="s">
+      <c r="C71" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="E71" s="13" t="s">
+      <c r="D71" s="14" t="s">
         <v>168</v>
       </c>
+      <c r="E71" s="14" t="s">
+        <v>169</v>
+      </c>
       <c r="F71" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H71" s="3"/>
-      <c r="I71" s="15"/>
-      <c r="J71" s="15"/>
-    </row>
-    <row r="72" s="16" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I71" s="20"/>
+      <c r="J71" s="20"/>
+    </row>
+    <row r="72" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
-      <c r="C72" s="13"/>
-      <c r="D72" s="13"/>
-      <c r="E72" s="13"/>
+      <c r="C72" s="14"/>
+      <c r="D72" s="14"/>
+      <c r="E72" s="14"/>
       <c r="F72" s="3"/>
       <c r="G72" s="3"/>
       <c r="H72" s="3"/>
-      <c r="I72" s="15"/>
-      <c r="J72" s="15"/>
-    </row>
-    <row r="73" s="16" customFormat="true" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I72" s="20"/>
+      <c r="J72" s="20"/>
+    </row>
+    <row r="73" s="21" customFormat="true" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="C73" s="13" t="s">
         <v>172</v>
       </c>
-      <c r="D73" s="13" t="s">
+      <c r="C73" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="E73" s="13" t="s">
+      <c r="D73" s="14" t="s">
         <v>174</v>
       </c>
+      <c r="E73" s="14" t="s">
+        <v>175</v>
+      </c>
       <c r="F73" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H73" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="I73" s="15"/>
-      <c r="J73" s="15"/>
-    </row>
-    <row r="74" s="16" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>178</v>
+      </c>
+      <c r="I73" s="20"/>
+      <c r="J73" s="20"/>
+    </row>
+    <row r="74" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="3"/>
       <c r="B74" s="3"/>
-      <c r="C74" s="13"/>
-      <c r="D74" s="13"/>
-      <c r="E74" s="13"/>
+      <c r="C74" s="14"/>
+      <c r="D74" s="14"/>
+      <c r="E74" s="14"/>
       <c r="F74" s="3"/>
       <c r="G74" s="3"/>
       <c r="H74" s="3"/>
-      <c r="I74" s="15"/>
-      <c r="J74" s="15"/>
-    </row>
-    <row r="75" customFormat="false" ht="86.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I74" s="20"/>
+      <c r="J74" s="20"/>
+    </row>
+    <row r="75" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="C75" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="D75" s="9" t="s">
+      <c r="C75" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="E75" s="9"/>
-      <c r="F75" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="G75" s="9" t="s">
+      <c r="D75" s="10" t="s">
         <v>181</v>
       </c>
+      <c r="E75" s="10"/>
+      <c r="F75" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="G75" s="10" t="s">
+        <v>182</v>
+      </c>
       <c r="H75" s="3"/>
-      <c r="I75" s="15"/>
-      <c r="J75" s="15"/>
-    </row>
-    <row r="76" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I75" s="20"/>
+      <c r="J75" s="20"/>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="3"/>
       <c r="B76" s="3"/>
       <c r="C76" s="1"/>
@@ -2656,30 +2913,30 @@
       <c r="F76" s="3"/>
       <c r="G76" s="3"/>
       <c r="H76" s="3"/>
-      <c r="I76" s="15"/>
-      <c r="J76" s="15"/>
-    </row>
-    <row r="77" customFormat="false" ht="374.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I76" s="20"/>
+      <c r="J76" s="20"/>
+    </row>
+    <row r="77" customFormat="false" ht="292.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="C77" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="D77" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="E77" s="9"/>
+      <c r="C77" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="D77" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="E77" s="10"/>
       <c r="F77" s="3"/>
       <c r="G77" s="3"/>
       <c r="H77" s="3"/>
-      <c r="I77" s="15"/>
-      <c r="J77" s="15"/>
-    </row>
-    <row r="78" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I77" s="20"/>
+      <c r="J77" s="20"/>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="3"/>
       <c r="B78" s="3"/>
       <c r="C78" s="1"/>
@@ -2688,64 +2945,64 @@
       <c r="F78" s="3"/>
       <c r="G78" s="3"/>
       <c r="H78" s="3"/>
-      <c r="I78" s="15"/>
-      <c r="J78" s="15"/>
-    </row>
-    <row r="79" customFormat="false" ht="201.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I78" s="20"/>
+      <c r="J78" s="20"/>
+    </row>
+    <row r="79" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B79" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="C79" s="9" t="s">
+      <c r="B79" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="D79" s="9"/>
-      <c r="E79" s="9"/>
-      <c r="F79" s="9"/>
-      <c r="G79" s="9" t="s">
+      <c r="C79" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="H79" s="9"/>
-    </row>
-    <row r="80" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D79" s="10"/>
+      <c r="E79" s="10"/>
+      <c r="F79" s="10"/>
+      <c r="G79" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="H79" s="10"/>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="7"/>
-      <c r="B80" s="9"/>
-      <c r="C80" s="9"/>
-      <c r="D80" s="9"/>
-      <c r="E80" s="9"/>
-      <c r="F80" s="9"/>
-      <c r="G80" s="9"/>
-      <c r="H80" s="9"/>
-    </row>
-    <row r="81" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B80" s="10"/>
+      <c r="C80" s="10"/>
+      <c r="D80" s="10"/>
+      <c r="E80" s="10"/>
+      <c r="F80" s="10"/>
+      <c r="G80" s="10"/>
+      <c r="H80" s="10"/>
+    </row>
+    <row r="81" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B81" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="C81" s="9" t="s">
+      <c r="B81" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="D81" s="9" t="s">
+      <c r="C81" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="E81" s="9" t="s">
+      <c r="D81" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="F81" s="9" t="s">
+      <c r="E81" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="G81" s="9" t="s">
+      <c r="F81" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="H81" s="9" t="s">
+      <c r="G81" s="10" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="82" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H81" s="10" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="4"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -2755,202 +3012,262 @@
       <c r="G82" s="1"/>
       <c r="H82" s="1"/>
     </row>
-    <row r="83" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="3"/>
       <c r="B83" s="3"/>
-      <c r="C83" s="13"/>
-      <c r="D83" s="13"/>
-      <c r="E83" s="13"/>
+      <c r="C83" s="14"/>
+      <c r="D83" s="14"/>
+      <c r="E83" s="14"/>
       <c r="F83" s="3"/>
       <c r="G83" s="3"/>
       <c r="H83" s="3"/>
-      <c r="I83" s="15"/>
-      <c r="J83" s="15"/>
-    </row>
-    <row r="84" s="19" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="85" s="4" customFormat="true" ht="247.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I83" s="20"/>
+      <c r="J83" s="20"/>
+    </row>
+    <row r="84" s="25" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="85" s="4" customFormat="true" ht="236.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E85" s="4" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="G85" s="4" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="H85" s="4" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="86" s="4" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="87" s="7" customFormat="true" ht="214.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="86" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="87" s="7" customFormat="true" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D87" s="7" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E87" s="7" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="F87" s="7" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="G87" s="7" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="H87" s="7" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="88" s="7" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="89" s="7" customFormat="true" ht="236.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="88" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="89" s="7" customFormat="true" ht="191.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D89" s="7" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E89" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="F89" s="7" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="G89" s="7" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="7"/>
-      <c r="B90" s="9"/>
-      <c r="C90" s="9"/>
-      <c r="D90" s="9"/>
+      <c r="B90" s="10"/>
+      <c r="C90" s="10"/>
+      <c r="D90" s="10"/>
       <c r="E90" s="7"/>
-      <c r="F90" s="9"/>
-      <c r="G90" s="9"/>
-      <c r="H90" s="9"/>
+      <c r="F90" s="10"/>
+      <c r="G90" s="10"/>
+      <c r="H90" s="10"/>
     </row>
     <row r="91" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B91" s="9" t="s">
-        <v>214</v>
-      </c>
-      <c r="C91" s="9" t="s">
+      <c r="B91" s="10" t="s">
         <v>215</v>
       </c>
-      <c r="D91" s="9" t="s">
+      <c r="C91" s="10" t="s">
         <v>216</v>
       </c>
+      <c r="D91" s="10" t="s">
+        <v>217</v>
+      </c>
       <c r="E91" s="7" t="s">
-        <v>217</v>
-      </c>
-      <c r="F91" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="G91" s="9" t="s">
+      <c r="F91" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="H91" s="9" t="s">
+      <c r="G91" s="10" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="92" s="7" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="H91" s="10" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="92" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="93" s="7" customFormat="true" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D93" s="7" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="E93" s="7" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="F93" s="7" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="G93" s="7" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="H93" s="7" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="94" s="7" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="95" s="7" customFormat="true" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="94" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="95" s="7" customFormat="true" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C95" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D95" s="7" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E95" s="7" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="F95" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="H95" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="96" s="11" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="96" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="97" s="4" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E97" s="7" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>225</v>
+      </c>
+    </row>
+    <row r="99" s="27" customFormat="true" ht="54.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A99" s="26" t="s">
+        <v>236</v>
+      </c>
+      <c r="B99" s="26"/>
+      <c r="C99" s="26"/>
+      <c r="D99" s="26"/>
+      <c r="E99" s="26"/>
+      <c r="F99" s="26"/>
+      <c r="G99" s="26"/>
+      <c r="H99" s="26"/>
+      <c r="I99" s="26"/>
+    </row>
+    <row r="101" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B101" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="D101" s="28" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B103" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="D103" s="28" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B105" s="28" t="s">
+        <v>241</v>
+      </c>
+      <c r="D105" s="0" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B107" s="28" t="s">
+        <v>243</v>
+      </c>
+      <c r="D107" s="0" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="109" s="25" customFormat="true" ht="337.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B109" s="25" t="s">
+        <v>245</v>
+      </c>
+      <c r="C109" s="25" t="s">
+        <v>246</v>
+      </c>
+      <c r="D109" s="25" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B111" s="0" t="s">
+        <v>248</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>